<commit_message>
update auto param and statistic
</commit_message>
<xml_diff>
--- a/file/output/py_Digital_BCL_12.0.xlsx
+++ b/file/output/py_Digital_BCL_12.0.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="variables" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="correlation" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="corr_pvalue" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="variables" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="correlation" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="corr_pvalue" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -11432,7 +11432,7 @@
         <v>2.686923792847445e-09</v>
       </c>
       <c r="M3" t="n">
-        <v>2.154282552255061e-08</v>
+        <v>2.154282552255116e-08</v>
       </c>
     </row>
     <row r="4">
@@ -11543,7 +11543,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>1.252941428879264e-232</v>
+        <v>1.252941428884352e-232</v>
       </c>
       <c r="H6" t="n">
         <v>0.9837922281374203</v>
@@ -11583,7 +11583,7 @@
         <v>2.981136276824765e-259</v>
       </c>
       <c r="F7" t="n">
-        <v>1.252941428879264e-232</v>
+        <v>1.252941428884352e-232</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
@@ -11601,7 +11601,7 @@
         <v>0.3828848220481738</v>
       </c>
       <c r="L7" t="n">
-        <v>0.08560424293786352</v>
+        <v>0.08560424293786417</v>
       </c>
       <c r="M7" t="n">
         <v>0.07133022891059719</v>
@@ -11641,7 +11641,7 @@
         <v>8.567317451804669e-20</v>
       </c>
       <c r="K8" t="n">
-        <v>4.646426098010521e-16</v>
+        <v>4.646426098010691e-16</v>
       </c>
       <c r="L8" t="n">
         <v>6.784874775059351e-16</v>
@@ -11681,13 +11681,13 @@
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>9.435393262408734e-06</v>
+        <v>9.435393262408852e-06</v>
       </c>
       <c r="K9" t="n">
         <v>0.001489347042742114</v>
       </c>
       <c r="L9" t="n">
-        <v>9.422647761351747e-09</v>
+        <v>9.422647761351499e-09</v>
       </c>
       <c r="M9" t="n">
         <v>1.532956816780747e-06</v>
@@ -11721,7 +11721,7 @@
         <v>8.567317451804669e-20</v>
       </c>
       <c r="I10" t="n">
-        <v>9.435393262408734e-06</v>
+        <v>9.435393262408852e-06</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -11733,7 +11733,7 @@
         <v>5.429004327700111e-64</v>
       </c>
       <c r="M10" t="n">
-        <v>1.811075299323454e-51</v>
+        <v>1.811075299323263e-51</v>
       </c>
     </row>
     <row r="11">
@@ -11761,7 +11761,7 @@
         <v>0.3828848220481738</v>
       </c>
       <c r="H11" t="n">
-        <v>4.646426098010521e-16</v>
+        <v>4.646426098010691e-16</v>
       </c>
       <c r="I11" t="n">
         <v>0.001489347042742114</v>
@@ -11801,13 +11801,13 @@
         <v>0.06843650122658781</v>
       </c>
       <c r="G12" t="n">
-        <v>0.08560424293786352</v>
+        <v>0.08560424293786417</v>
       </c>
       <c r="H12" t="n">
         <v>6.784874775059351e-16</v>
       </c>
       <c r="I12" t="n">
-        <v>9.422647761351747e-09</v>
+        <v>9.422647761351499e-09</v>
       </c>
       <c r="J12" t="n">
         <v>5.429004327700111e-64</v>
@@ -11832,7 +11832,7 @@
         <v>4.835907653497078e-08</v>
       </c>
       <c r="C13" t="n">
-        <v>2.154282552255061e-08</v>
+        <v>2.154282552255116e-08</v>
       </c>
       <c r="D13" t="n">
         <v>4.125894595241929e-08</v>
@@ -11853,7 +11853,7 @@
         <v>1.532956816780747e-06</v>
       </c>
       <c r="J13" t="n">
-        <v>1.811075299323454e-51</v>
+        <v>1.811075299323263e-51</v>
       </c>
       <c r="K13" t="n">
         <v>3.299744437900828e-20</v>

</xml_diff>